<commit_message>
Compilando para la version final
</commit_message>
<xml_diff>
--- a/Budget/Budget ERC.xlsx
+++ b/Budget/Budget ERC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11009"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/Documents/11-Funding/ERC/Budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3C16AF-999B-B94F-994B-99AD28DD5F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC3EB50-6F89-C04E-B5CC-81B02D6D3704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="22540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full project duration" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <r>
       <t xml:space="preserve">Total Requested EU Contribution </t>
@@ -252,9 +252,6 @@
     <t xml:space="preserve">Equipment </t>
   </si>
   <si>
-    <t>Consumables (incl. Fieldwork and animal costs)</t>
-  </si>
-  <si>
     <t>Publications (including Open Access fees 
 &amp; dissemination), etc.</t>
   </si>
@@ -326,6 +323,36 @@
   </si>
   <si>
     <t xml:space="preserve"> &gt;= 10 ans</t>
+  </si>
+  <si>
+    <t>Postdoc 1</t>
+  </si>
+  <si>
+    <t>Postdoc 2</t>
+  </si>
+  <si>
+    <t>Postdoc 3</t>
+  </si>
+  <si>
+    <t>PhD1</t>
+  </si>
+  <si>
+    <t>PhD2</t>
+  </si>
+  <si>
+    <t>PhD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumables </t>
+  </si>
+  <si>
+    <t>Travels ( Conf/year *3 persones )</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Ingenieur d'Etudes</t>
   </si>
 </sst>
 </file>
@@ -894,7 +921,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1124,9 +1151,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1310,6 +1334,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1318,12 +1348,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1724,14 +1748,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Feuil1">
     <tabColor rgb="FFC00000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="91" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="129" zoomScalePageLayoutView="91" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1748,12 +1772,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="158" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="160"/>
+      <c r="C1" s="157" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="159"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="2:8" ht="19" x14ac:dyDescent="0.25">
@@ -1768,11 +1792,11 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="155" t="s">
+      <c r="B5" s="154" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="156"/>
-      <c r="D5" s="157"/>
+      <c r="C5" s="155"/>
+      <c r="D5" s="156"/>
       <c r="E5" s="27"/>
       <c r="F5" s="26" t="s">
         <v>12</v>
@@ -1780,10 +1804,10 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="161" t="s">
+      <c r="B6" s="160" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="164"/>
+      <c r="C6" s="163"/>
       <c r="D6" s="37" t="s">
         <v>43</v>
       </c>
@@ -1794,69 +1818,104 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="162"/>
-      <c r="C7" s="165"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="164"/>
       <c r="D7" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="75"/>
+      <c r="E7" s="75">
+        <v>45</v>
+      </c>
       <c r="F7" s="87">
-        <f>60000*5</f>
-        <v>300000</v>
+        <f>5518*E7</f>
+        <v>248310</v>
       </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="162"/>
-      <c r="C8" s="166"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="92"/>
+    <row r="8" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="161"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="94">
+        <v>24</v>
+      </c>
+      <c r="F8" s="92">
+        <f>50234*2</f>
+        <v>100468</v>
+      </c>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="162"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="92"/>
+    <row r="9" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="161"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="98" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="94">
+        <v>24</v>
+      </c>
+      <c r="F9" s="92">
+        <f>50234*2</f>
+        <v>100468</v>
+      </c>
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="162"/>
-      <c r="C10" s="166"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="92"/>
+      <c r="B10" s="161"/>
+      <c r="C10" s="165"/>
+      <c r="D10" s="98" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="94">
+        <v>24</v>
+      </c>
+      <c r="F10" s="92">
+        <v>0</v>
+      </c>
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="162"/>
-      <c r="C11" s="166"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="93"/>
+      <c r="B11" s="161"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="76">
+        <v>60</v>
+      </c>
+      <c r="F11" s="93">
+        <f>225000</f>
+        <v>225000</v>
+      </c>
       <c r="G11" s="55"/>
     </row>
     <row r="12" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="162"/>
-      <c r="C12" s="166"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="93"/>
+      <c r="B12" s="161"/>
+      <c r="C12" s="165"/>
+      <c r="D12" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="76">
+        <v>30</v>
+      </c>
+      <c r="F12" s="93">
+        <v>100000</v>
+      </c>
       <c r="G12" s="56"/>
     </row>
     <row r="13" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="162"/>
-      <c r="C13" s="166"/>
+      <c r="B13" s="161"/>
+      <c r="C13" s="165"/>
       <c r="D13" s="89"/>
       <c r="E13" s="88"/>
       <c r="F13" s="18"/>
       <c r="G13" s="56"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="162"/>
-      <c r="C14" s="165"/>
+      <c r="B14" s="161"/>
+      <c r="C14" s="164"/>
       <c r="D14" s="73" t="s">
         <v>16</v>
       </c>
@@ -1866,8 +1925,8 @@
       <c r="H14" s="51"/>
     </row>
     <row r="15" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="162"/>
-      <c r="C15" s="165"/>
+      <c r="B15" s="161"/>
+      <c r="C15" s="164"/>
       <c r="D15" s="90" t="s">
         <v>37</v>
       </c>
@@ -1879,35 +1938,53 @@
       <c r="H15" s="50"/>
     </row>
     <row r="16" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="162"/>
-      <c r="C16" s="165"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="93"/>
+      <c r="B16" s="161"/>
+      <c r="C16" s="164"/>
+      <c r="D16" s="91" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="96">
+        <v>36</v>
+      </c>
+      <c r="F16" s="93">
+        <v>119000</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="50"/>
     </row>
     <row r="17" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="162"/>
-      <c r="C17" s="165"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="93"/>
+      <c r="B17" s="161"/>
+      <c r="C17" s="164"/>
+      <c r="D17" s="91" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="96">
+        <v>36</v>
+      </c>
+      <c r="F17" s="93">
+        <v>119000</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="50"/>
     </row>
     <row r="18" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="162"/>
-      <c r="C18" s="165"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="93"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="91" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="97">
+        <v>36</v>
+      </c>
+      <c r="F18" s="93">
+        <v>0</v>
+      </c>
       <c r="G18" s="47"/>
       <c r="H18" s="49"/>
     </row>
     <row r="19" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="162"/>
-      <c r="C19" s="165"/>
+      <c r="B19" s="161"/>
+      <c r="C19" s="164"/>
       <c r="D19" s="24"/>
       <c r="E19" s="77"/>
       <c r="F19" s="83"/>
@@ -1915,8 +1992,8 @@
       <c r="H19" s="49"/>
     </row>
     <row r="20" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="162"/>
-      <c r="C20" s="167"/>
+      <c r="B20" s="161"/>
+      <c r="C20" s="166"/>
       <c r="D20" s="84"/>
       <c r="E20" s="81"/>
       <c r="F20" s="18"/>
@@ -1924,55 +2001,61 @@
       <c r="H20" s="49"/>
     </row>
     <row r="21" spans="2:8" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="162"/>
-      <c r="C21" s="168" t="s">
+      <c r="B21" s="161"/>
+      <c r="C21" s="167" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="169"/>
+      <c r="D21" s="168"/>
       <c r="E21" s="23"/>
       <c r="F21" s="12">
-        <f>SUM(F14:F20)</f>
-        <v>0</v>
+        <f>SUM(F6:F20)</f>
+        <v>1012246</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="48"/>
     </row>
     <row r="22" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="162"/>
-      <c r="C22" s="170" t="s">
+      <c r="B22" s="161"/>
+      <c r="C22" s="169" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="171"/>
+      <c r="D22" s="170"/>
       <c r="E22" s="20"/>
       <c r="F22" s="18"/>
       <c r="G22" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="162"/>
+    <row r="23" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="161"/>
       <c r="C23" s="22"/>
-      <c r="D23" s="21"/>
+      <c r="D23" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E23" s="20"/>
-      <c r="F23" s="18"/>
+      <c r="F23" s="18">
+        <v>50000</v>
+      </c>
       <c r="G23" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="162"/>
-      <c r="C24" s="170" t="s">
+      <c r="B24" s="161"/>
+      <c r="C24" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="171"/>
+      <c r="D24" s="170"/>
       <c r="E24" s="19"/>
-      <c r="F24" s="18"/>
+      <c r="F24" s="18">
+        <v>110000</v>
+      </c>
       <c r="G24" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="162"/>
+      <c r="B25" s="161"/>
       <c r="C25" s="17"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1980,106 +2063,122 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="162"/>
-      <c r="C26" s="172" t="s">
+      <c r="B26" s="161"/>
+      <c r="C26" s="171" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="18">
+        <v>40000</v>
+      </c>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="2:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="161"/>
+      <c r="C27" s="164"/>
+      <c r="D27" s="85" t="s">
         <v>47</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" spans="2:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="162"/>
-      <c r="C27" s="165"/>
-      <c r="D27" s="85" t="s">
-        <v>48</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="18">
-        <f>20000</f>
-        <v>20000</v>
+        <f>24000</f>
+        <v>24000</v>
       </c>
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="162"/>
-      <c r="C28" s="165"/>
+      <c r="B28" s="161"/>
+      <c r="C28" s="164"/>
       <c r="D28" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="15"/>
-      <c r="F28" s="8"/>
+      <c r="F28" s="8">
+        <v>15000</v>
+      </c>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="2:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="163"/>
-      <c r="C29" s="168" t="s">
+      <c r="B29" s="162"/>
+      <c r="C29" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="169"/>
+      <c r="D29" s="168"/>
       <c r="E29" s="13"/>
-      <c r="F29" s="12"/>
+      <c r="F29" s="12">
+        <f>SUM(F22:F28)</f>
+        <v>239000</v>
+      </c>
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="2:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="149" t="s">
+      <c r="B30" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="150"/>
-      <c r="D30" s="151"/>
+      <c r="C30" s="149"/>
+      <c r="D30" s="150"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="8"/>
+      <c r="F30" s="8">
+        <f xml:space="preserve"> SUM(F21+F29)</f>
+        <v>1251246</v>
+      </c>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="2:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="152" t="s">
+      <c r="B31" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="153"/>
-      <c r="D31" s="154"/>
+      <c r="C31" s="152"/>
+      <c r="D31" s="153"/>
       <c r="E31" s="11"/>
-      <c r="F31" s="10"/>
+      <c r="F31" s="10">
+        <f>0.25*F30</f>
+        <v>312811.5</v>
+      </c>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="2:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="149" t="s">
+      <c r="B32" s="148" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="150"/>
-      <c r="D32" s="151"/>
+      <c r="C32" s="149"/>
+      <c r="D32" s="150"/>
       <c r="E32" s="9"/>
       <c r="F32" s="8"/>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="140" t="s">
+      <c r="B33" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="141"/>
-      <c r="D33" s="142"/>
+      <c r="C33" s="140"/>
+      <c r="D33" s="141"/>
       <c r="E33" s="7"/>
       <c r="F33" s="6"/>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="143" t="s">
+      <c r="B34" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="144"/>
-      <c r="D34" s="145"/>
+      <c r="C34" s="143"/>
+      <c r="D34" s="144"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="3"/>
+      <c r="F34" s="3">
+        <f xml:space="preserve"> SUM(F30:F33)</f>
+        <v>1564057.5</v>
+      </c>
       <c r="G34" s="62"/>
     </row>
     <row r="35" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="146" t="s">
+      <c r="B35" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="147"/>
-      <c r="D35" s="148"/>
+      <c r="C35" s="146"/>
+      <c r="D35" s="147"/>
       <c r="E35" s="4"/>
       <c r="F35" s="78"/>
       <c r="G35" s="2"/>
@@ -2120,10 +2219,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2138,380 +2238,380 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="86" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
     </row>
     <row r="2" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="100" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="103"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="104"/>
-    </row>
-    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="106"/>
+    </row>
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="174" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="107"/>
-    </row>
-    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="173" t="s">
+      <c r="B6" s="175"/>
+      <c r="C6" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="108" t="s">
+      <c r="D6" s="108" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="109" t="s">
+      <c r="E6" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="110" t="s">
+      <c r="F6" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="111" t="s">
+      <c r="G6" s="111"/>
+      <c r="H6" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="113" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="175"/>
-      <c r="B7" s="175"/>
-      <c r="C7" s="114">
+      <c r="A7" s="176"/>
+      <c r="B7" s="176"/>
+      <c r="C7" s="113">
         <v>1768.55</v>
       </c>
-      <c r="D7" s="115">
+      <c r="D7" s="114">
         <f>C7*1.42</f>
         <v>2511.3409999999999</v>
       </c>
-      <c r="E7" s="116">
+      <c r="E7" s="115">
         <v>12</v>
       </c>
-      <c r="F7" s="117">
+      <c r="F7" s="116">
         <f>D7*E7</f>
         <v>30136.091999999997</v>
       </c>
-      <c r="G7" s="112"/>
-      <c r="H7" s="118">
+      <c r="G7" s="111"/>
+      <c r="H7" s="117">
         <f>C7*0.79</f>
         <v>1397.1545000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="119" t="s">
-        <v>60</v>
+      <c r="A8" s="118" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="119"/>
+      <c r="A9" s="118"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="119"/>
+      <c r="A10" s="118"/>
     </row>
     <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="100" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="101"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="103"/>
+    </row>
+    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="104" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="106"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="102"/>
-      <c r="C12" s="102"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="104"/>
-    </row>
-    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="105" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="106"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="107"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="120" t="s">
+    </row>
+    <row r="17" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="120" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="121" t="s">
+      <c r="B17" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="122" t="s">
+      <c r="C17" s="122" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="123" t="s">
+      <c r="D17" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="124" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="125" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="126"/>
+      <c r="H17" s="127" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="172" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="124" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="125" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="126" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="127"/>
-      <c r="H17" s="128" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="176" t="s">
+      <c r="B18" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="129" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="130">
+      <c r="C18" s="129">
         <v>2130</v>
       </c>
-      <c r="D18" s="131">
+      <c r="D18" s="130">
         <f>C18*1.42</f>
         <v>3024.6</v>
       </c>
-      <c r="E18" s="132">
+      <c r="E18" s="131">
         <v>12</v>
       </c>
-      <c r="F18" s="133">
+      <c r="F18" s="132">
         <f>D18*E18</f>
         <v>36295.199999999997</v>
       </c>
-      <c r="G18" s="134"/>
-      <c r="H18" s="135">
+      <c r="G18" s="133"/>
+      <c r="H18" s="134">
         <f>C18*0.79</f>
         <v>1682.7</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="177"/>
-      <c r="B19" s="129" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="130">
+      <c r="A19" s="173"/>
+      <c r="B19" s="128" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="129">
         <v>2948</v>
       </c>
-      <c r="D19" s="131">
+      <c r="D19" s="130">
         <f>C19*1.42</f>
         <v>4186.16</v>
       </c>
-      <c r="E19" s="132">
+      <c r="E19" s="131">
         <v>12</v>
       </c>
-      <c r="F19" s="133">
+      <c r="F19" s="132">
         <f>D19*E19</f>
         <v>50233.919999999998</v>
       </c>
-      <c r="G19" s="134"/>
-      <c r="H19" s="135">
+      <c r="G19" s="133"/>
+      <c r="H19" s="134">
         <f>C19*0.79</f>
         <v>2328.92</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="136"/>
-      <c r="B20" s="134"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
+      <c r="A20" s="135"/>
+      <c r="B20" s="133"/>
+      <c r="C20" s="133"/>
+      <c r="D20" s="133"/>
       <c r="E20" s="61"/>
-      <c r="F20" s="134"/>
-      <c r="G20" s="134"/>
-      <c r="H20" s="137"/>
+      <c r="F20" s="133"/>
+      <c r="G20" s="133"/>
+      <c r="H20" s="136"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="176" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="129" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="130">
+      <c r="A21" s="172" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="129">
         <v>2300</v>
       </c>
-      <c r="D21" s="131">
+      <c r="D21" s="130">
         <f>C21*1.42</f>
         <v>3266</v>
       </c>
-      <c r="E21" s="132">
+      <c r="E21" s="131">
         <v>12</v>
       </c>
-      <c r="F21" s="133">
+      <c r="F21" s="132">
         <f>D21*E21</f>
         <v>39192</v>
       </c>
-      <c r="G21" s="134"/>
-      <c r="H21" s="135">
+      <c r="G21" s="133"/>
+      <c r="H21" s="134">
         <f>C21*0.79</f>
         <v>1817</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="177"/>
-      <c r="B22" s="129" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="130">
+      <c r="A22" s="173"/>
+      <c r="B22" s="128" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="129">
         <v>3545</v>
       </c>
-      <c r="D22" s="131">
+      <c r="D22" s="130">
         <f>C22*1.42</f>
         <v>5033.8999999999996</v>
       </c>
-      <c r="E22" s="132">
+      <c r="E22" s="131">
         <v>12</v>
       </c>
-      <c r="F22" s="133">
+      <c r="F22" s="132">
         <f>D22*E22</f>
         <v>60406.799999999996</v>
       </c>
-      <c r="G22" s="134"/>
-      <c r="H22" s="135">
+      <c r="G22" s="133"/>
+      <c r="H22" s="134">
         <f>C22*0.79</f>
         <v>2800.55</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="136"/>
-      <c r="B23" s="134"/>
-      <c r="C23" s="134"/>
-      <c r="D23" s="134"/>
+      <c r="A23" s="135"/>
+      <c r="B23" s="133"/>
+      <c r="C23" s="133"/>
+      <c r="D23" s="133"/>
       <c r="E23" s="61"/>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="137"/>
+      <c r="F23" s="133"/>
+      <c r="G23" s="133"/>
+      <c r="H23" s="136"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="176" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="129" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="130">
+      <c r="A24" s="172" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="129">
         <v>2650</v>
       </c>
-      <c r="D24" s="131">
+      <c r="D24" s="130">
         <f>C24*1.42</f>
         <v>3763</v>
       </c>
-      <c r="E24" s="132">
+      <c r="E24" s="131">
         <v>12</v>
       </c>
-      <c r="F24" s="133">
+      <c r="F24" s="132">
         <f>D24*E24</f>
         <v>45156</v>
       </c>
-      <c r="G24" s="134"/>
-      <c r="H24" s="135">
+      <c r="G24" s="133"/>
+      <c r="H24" s="134">
         <f>C24*0.79</f>
         <v>2093.5</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="177"/>
-      <c r="B25" s="129" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="130">
+      <c r="A25" s="173"/>
+      <c r="B25" s="128" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="129">
         <v>3886</v>
       </c>
-      <c r="D25" s="131">
+      <c r="D25" s="130">
         <f>C25*1.42</f>
         <v>5518.12</v>
       </c>
-      <c r="E25" s="132">
+      <c r="E25" s="131">
         <v>12</v>
       </c>
-      <c r="F25" s="133">
+      <c r="F25" s="132">
         <f>D25*E25</f>
         <v>66217.440000000002</v>
       </c>
-      <c r="G25" s="134"/>
-      <c r="H25" s="135">
+      <c r="G25" s="133"/>
+      <c r="H25" s="134">
         <f>C25*0.79</f>
         <v>3069.94</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="136"/>
-      <c r="B26" s="134"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="134"/>
+      <c r="A26" s="135"/>
+      <c r="B26" s="133"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
       <c r="E26" s="61"/>
-      <c r="F26" s="134"/>
-      <c r="G26" s="134"/>
-      <c r="H26" s="137"/>
+      <c r="F26" s="133"/>
+      <c r="G26" s="133"/>
+      <c r="H26" s="136"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="176" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="129" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="130">
+      <c r="A27" s="172" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="129">
         <v>3160</v>
       </c>
-      <c r="D27" s="131">
+      <c r="D27" s="130">
         <f>C27*1.42</f>
         <v>4487.2</v>
       </c>
-      <c r="E27" s="132">
+      <c r="E27" s="131">
         <v>12</v>
       </c>
-      <c r="F27" s="133">
+      <c r="F27" s="132">
         <f>D27*E27</f>
         <v>53846.399999999994</v>
       </c>
-      <c r="G27" s="134"/>
-      <c r="H27" s="135">
+      <c r="G27" s="133"/>
+      <c r="H27" s="134">
         <f>C27*0.79</f>
         <v>2496.4</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="177"/>
-      <c r="B28" s="129" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="130">
+      <c r="A28" s="173"/>
+      <c r="B28" s="128" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="129">
         <v>4184</v>
       </c>
-      <c r="D28" s="131">
+      <c r="D28" s="130">
         <f>C28*1.42</f>
         <v>5941.28</v>
       </c>
-      <c r="E28" s="132">
+      <c r="E28" s="131">
         <v>12</v>
       </c>
-      <c r="F28" s="133">
+      <c r="F28" s="132">
         <f>D28*E28</f>
         <v>71295.360000000001</v>
       </c>
-      <c r="G28" s="138"/>
-      <c r="H28" s="139">
+      <c r="G28" s="137"/>
+      <c r="H28" s="138">
         <f>C28*0.79</f>
         <v>3305.36</v>
       </c>
@@ -2537,6 +2637,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2560,7 +2661,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="86" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="86"/>
     </row>
@@ -2582,10 +2683,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Feuil4"/>
   <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2648,10 +2750,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Feuil5"/>
   <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2764,7 +2867,7 @@
       </c>
       <c r="C18" s="65">
         <f>'Full project duration'!$F$31</f>
-        <v>0</v>
+        <v>312811.5</v>
       </c>
       <c r="D18" s="54"/>
       <c r="E18" s="54"/>
@@ -2786,7 +2889,7 @@
       </c>
       <c r="C20" s="74">
         <f>C18+C19</f>
-        <v>0</v>
+        <v>312811.5</v>
       </c>
       <c r="D20" s="68">
         <f>SUM(C3:C8)</f>
@@ -2794,7 +2897,7 @@
       </c>
       <c r="E20" s="70">
         <f>C20-D20</f>
-        <v>-130600</v>
+        <v>182211.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>